<commit_message>
Data verification in progress
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/SelfRasScreenerSubmissionScenarios.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/SelfRasScreenerSubmissionScenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juarezds/Desktop/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37AB4F9-928D-7243-B97E-A379381A5FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C333871-F360-5740-AD2E-D292584F5E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34480" yWindow="-1260" windowWidth="30240" windowHeight="17440" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
@@ -612,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated SEER tags and Senario2 for CHARMS RAS Screener
</commit_message>
<xml_diff>
--- a/src/test/java/ServiceNow/CHARMS/Resources/SelfRasScreenerSubmissionScenarios.xlsx
+++ b/src/test/java/ServiceNow/CHARMS/Resources/SelfRasScreenerSubmissionScenarios.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juarezds/Desktop/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bucurgb/IdeaProjects/CBIIT-Test-Automation/src/test/java/ServiceNow/CHARMS/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37AB4F9-928D-7243-B97E-A379381A5FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7755886-EA94-0745-A7D5-0F25C119748A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34480" yWindow="-1260" windowWidth="30240" windowHeight="17440" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
+    <workbookView xWindow="102400" yWindow="180" windowWidth="51200" windowHeight="28300" xr2:uid="{54739BCC-024D-1B43-9BD3-233381306DEA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scenario1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenario2" sheetId="2" r:id="rId1"/>
+    <sheet name="Scenario1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
   <si>
     <t>Question</t>
   </si>
@@ -222,6 +223,77 @@
   </si>
   <si>
     <t>What are the main reasons for participating in this study?  Select all that apply.  Please elaborate on the reason in the corresponding textbox. Other reason</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Martian</t>
+  </si>
+  <si>
+    <t>Race text box</t>
+  </si>
+  <si>
+    <t>Family Advocacy Group</t>
+  </si>
+  <si>
+    <t>Non-cancerous tumors</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with the following conditions?  Select all that apply.  If you do not see the exact condition diagnosed, please select the closest answer. Option 9</t>
+  </si>
+  <si>
+    <t>Have you ever been diagnosed with the following conditions?  Select all that apply.  If you do not see the exact condition diagnosed, please select the closest answer. Option 10</t>
+  </si>
+  <si>
+    <t>Lymphedema</t>
+  </si>
+  <si>
+    <t>Neurablastoma</t>
+  </si>
+  <si>
+    <t>Bug. Year of diagnosis and age  should go with birthday date.</t>
+  </si>
+  <si>
+    <t>Bug. You should not be able to move forward without comleting Other field</t>
+  </si>
+  <si>
+    <t>Please complete the box below by selecting which primary cancers were diagnosed and at what age and year they occurred. If cancer spread from one place to another, please only indicate the original cancers and not the number of sites where cancer spread.
+Age at diagnosis</t>
+  </si>
+  <si>
+    <t>Please complete the box below by selecting which primary cancers were diagnosed and at what age and year they occurred. If cancer spread from one place to another, please only indicate the original cancers and not the number of sites where cancer spread.
+Year at diagnosis</t>
+  </si>
+  <si>
+    <t>Please complete the box below by selecting which primary cancers were diagnosed and at what age and year they occurred. If cancer spread from one place to another, please only indicate the original cancers and not the number of sites where cancer spread.
+Cancer Type</t>
+  </si>
+  <si>
+    <t>Please complete the box below by selecting which primary cancers were diagnosed and at what age and year they occurred. If cancer spread from one place to another, please only indicate the original cancers and not the number of sites where cancer spread.
+Curently receiving treatment</t>
+  </si>
+  <si>
+    <t>GeorgeTest</t>
+  </si>
+  <si>
+    <t>BucurTest</t>
+  </si>
+  <si>
+    <t>automatedTestGeorge@email.com</t>
+  </si>
+  <si>
+    <t>The selection should be only one check box. Multiple boxes can be checked. The checked boxes should be radio buttons.</t>
+  </si>
+  <si>
+    <t>What are the main reasons for participating in this study?  Select all that apply.  Please elaborate on the reason in the corresponding textbox.
+Other reason Text Box</t>
+  </si>
+  <si>
+    <t>More fields in the Native view and not enough in the form</t>
   </si>
 </sst>
 </file>
@@ -609,10 +681,391 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B08174-57EB-4C4A-A12B-17F5EA82D530}">
+  <dimension ref="A1:C45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <v>32964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4">
+        <v>22015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="4">
+        <v>15</v>
+      </c>
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B18" r:id="rId1" xr:uid="{DFB0DCAE-7F47-6349-92CC-F426262B8C9C}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{C11E052E-261B-0A4D-AF2E-9C67EFC2BCB7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AAA49E6-03DB-BC47-B34D-065780B05137}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>

</xml_diff>